<commit_message>
erro de navegação corrigido
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,8 +30,12 @@
       <color rgb="00FFFFFF"/>
       <sz val="12"/>
     </font>
+    <font>
+      <color rgb="00404040"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -44,8 +48,14 @@
         <bgColor rgb="00044F83"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00f2f2f2"/>
+        <bgColor rgb="00f2f2f2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -53,14 +63,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -427,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,6 +508,92 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>https://www.anchieta.es.gov.br/bootstrap/7l8u3v5</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+A notícia informa que a Prefeitura Municipal de Anchieta, no Espírito Santo, tem realizado diversas ações para melhorar a qualidade de vida na cidade. Entre elas estão o reforço na limpeza urbana, melhoria da iluminação pública e construção de novas ruas e calçadas. Também houve investimentos em educação com a construção de escolas e reformas nas unidades já existentes.</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>/noticias/governo-do-estado-anuncia-investimentos-em-infraestrutura
+Não tem.</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>/noticias/governo-investira-r-2-5-bilhoes-em-infraestrutura
+R$ 2,5 bilhões</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>/
+As principais localidades mencionadas neste link são Anchieta, São Mateus, Conceição da Barra, Linhares e Vila Velha.</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>y/conteudo
+O secretário de Estado da Agricultura, Pecuária e Abastecimento, Valter Bianchini.</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Sou da Verum Partners, uma empresa de consultoria atuante no mercado de infraestrutura, construção e gerenciamento de projetos. Soubemos que a Prefeitura Municipal de Anchieta irá ampliar o seu porto com investimentos na ordem de R$ 8 milhões. Este anúncio nos chamou atenção porque o investimento contempla a realização de obras estruturantes, desafio muito similar ao que temos nos envolvido e obtido resultados relevantes junto à nossos clientes. Pensando em ajudá-los a posicionar este projeto como um case de sucesso, gostaria de agendar uma rápida reunião contigo para apresentar como ajudamos outras organizações como a Prefeitura Municipal de Anchieta em projetos similares, compreender os seus desafios, bem como analisar se podemos trabalhar juntos.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>https://monitordomercado.com.br/noticias/40037-bunge-cia-tem-lucro-de-us-336-milhoes-no-4t22</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+A Bunge, uma companhia global de agronegócios, anunciou seu lucro no quarto trimestre de 2020 de US$ 336 milhões. O resultado foi impulsionado pela demanda por alimentos em todo o mundo durante a pandemia, que gerou um aumento das vendas e dos preços dos produtos. O lucro líquido do período foi 5 vezes maior do que no mesmo período do ano anterior. A receita operacional também cresceu 8%, para US$ 13 bilhões.</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Bunge</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+336 milhões.</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+As principais localidades mencionadas neste link são: Brasil, Estados Unidos, América Latina e Europa.</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Gregory Heckman, CEO da Bunge.</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Sou da Verum Partners, uma empresa de consultoria atuante no mercado de infraestrutura, construção e gerenciamento de projetos. Soubemos que a Bunge Cia teve um lucro de US$ 336 milhões no 4T22, segundo o anúncio feito pela empresa. Este anúncio nos chamou atenção porque o investimento contempla a realização de projetos estratégicos para o futuro da companhia, desafio muito similar ao que temos nos envolvido e obtido resultados relevantes junto à nossos clientes. Pensando em ajudá-los a posicionar este projeto como um case de sucesso, gostaria de agendar uma rápida reunião contigo para apresentar como ajudamos outras organizações como a Bunge Cia em projetos similares, compreender os seus desafios, bem como analisar se podemos trabalhar juntos.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>